<commit_message>
updated readme, added FR and EN json
</commit_message>
<xml_diff>
--- a/20251117_Sam_Translations_FR.xlsx
+++ b/20251117_Sam_Translations_FR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karel.dries\Downloads\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kadr\git\copilot_translations_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966B5937-70AC-4D0D-B466-3BE9259EED0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA1A8E5-710C-431D-9B24-D55901BEF309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,10 @@
     <t>'customEntity(cr93b_generatieveSam.entity.Arbeidsstatuut)'.Description</t>
   </si>
   <si>
+    <t>Hier vragen we naar het statuut van de klant; werknemer, werkloos of zelfstandig</t>
+  </si>
+  <si>
     <t>'customEntity(cr93b_generatieveSam.entity.Arbeidsstatuut)'.DisplayName</t>
-  </si>
-  <si>
-    <t>Arbeidsstatuut</t>
   </si>
   <si>
     <t>'customEntity(cr93b_generatieveSam.entity.Arbeidsstatuut)'.Entity.'closedListItem(NowrD8)'.DisplayName</t>
@@ -1643,7 +1643,7 @@
     <t>helanzorgwinkel.be/uitleendienst</t>
   </si>
   <si>
-    <t>Ici, nous demandons le statut du client : salarié, chômeur ou indépendant</t>
+    <t>test fr vertaling</t>
   </si>
 </sst>
 </file>
@@ -2030,15 +2030,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>525</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>